<commit_message>
update plantilla y favicon
</commit_message>
<xml_diff>
--- a/template/plantilla.xlsx
+++ b/template/plantilla.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sauls\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\web\codigo_barras\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4F9AA29B-2584-46A3-B975-CB49DFF1FE9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE558361-1B96-4CC4-8736-98C27D86B4A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{0D86A988-633D-44C1-A1B0-57BAE1D71C95}"/>
   </bookViews>
@@ -57,7 +57,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -65,13 +65,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF002060"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -86,8 +99,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -425,25 +441,30 @@
   <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="39.6328125" customWidth="1"/>
+    <col min="4" max="4" width="12.7265625" customWidth="1"/>
+    <col min="5" max="5" width="13.1796875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>